<commit_message>
code mới hôm nay. THêm tính năng thêm cuoc trò chuyện và hien thi ten nguoi dung
</commit_message>
<xml_diff>
--- a/New folder/Book1.xlsx
+++ b/New folder/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\VS code\js\CI gen 75\SS2\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\HOMEWORK-CI45-SS2\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB35306-154D-481A-9451-0576A6CF01F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A06670F-EA1A-4B9E-BE5C-48B0B3342AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B295C40F-EBA3-4D4C-874F-5B9BB3F8E95B}"/>
+    <workbookView xWindow="312" yWindow="540" windowWidth="17280" windowHeight="8964" xr2:uid="{B295C40F-EBA3-4D4C-874F-5B9BB3F8E95B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Nguyễn Đỗ Khánh</t>
   </si>
@@ -54,6 +54,42 @@
   </si>
   <si>
     <t>không nộp bài</t>
+  </si>
+  <si>
+    <t>nộp bài muộn  (BTVN: 11/08/2020)</t>
+  </si>
+  <si>
+    <t>Ngô Tiến Thuận</t>
+  </si>
+  <si>
+    <t>Đoàn Mạnh Cường</t>
+  </si>
+  <si>
+    <t>Minh Bếu</t>
+  </si>
+  <si>
+    <t>Nguyễn Trung Hiếu</t>
+  </si>
+  <si>
+    <t>Hùng Phùng</t>
+  </si>
+  <si>
+    <t>Vũ Thành Long</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiếu Bùi </t>
+  </si>
+  <si>
+    <t>Hiếu Nguyễn</t>
+  </si>
+  <si>
+    <t>Nguyen Tien Dung</t>
+  </si>
+  <si>
+    <t>Lê Hiếu</t>
   </si>
 </sst>
 </file>
@@ -95,11 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147A25B1-DEDC-4CB0-AE70-A26D25917899}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,9 +513,70 @@
       </c>
       <c r="C5" s="2"/>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:C5"/>
+    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>